<commit_message>
added more usability tests
</commit_message>
<xml_diff>
--- a/Usability_Tests/UB-Protocol Wettermonitor_T3_EW.xlsx
+++ b/Usability_Tests/UB-Protocol Wettermonitor_T3_EW.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\01_SG DS\Kompetenzen\gdv_GrundlagenDatenvisualisierung\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\FHNW\Kompetenzen\gdv_Fundamentals_Data_Viz\fhnw-ds-hs2020-gdv_data_visualization\Usability_Tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{827A06D5-A2A5-4D5A-8C2E-0BACF93EF24E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B9C4E44-2B56-4C69-A29C-29B00B5E6E91}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{3F1E84BA-F577-4401-86F6-6D87C2FA444C}"/>
+    <workbookView xWindow="1170" yWindow="1170" windowWidth="21600" windowHeight="11385" xr2:uid="{3F1E84BA-F577-4401-86F6-6D87C2FA444C}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -1059,6 +1059,7 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1146,7 +1147,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -1463,8 +1463,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0A6C56F-17AE-44D4-8CA9-39029899ABD2}">
   <dimension ref="B2:H45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I36" sqref="I36"/>
+    <sheetView tabSelected="1" topLeftCell="C17" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C36" sqref="C34:C36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1520,15 +1520,15 @@
       <c r="G5" s="10"/>
     </row>
     <row r="6" spans="2:8" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="30" t="s">
+      <c r="B6" s="31" t="s">
         <v>71</v>
       </c>
-      <c r="C6" s="31"/>
-      <c r="D6" s="31"/>
-      <c r="E6" s="31"/>
-      <c r="F6" s="31"/>
-      <c r="G6" s="31"/>
-      <c r="H6" s="32"/>
+      <c r="C6" s="32"/>
+      <c r="D6" s="32"/>
+      <c r="E6" s="32"/>
+      <c r="F6" s="32"/>
+      <c r="G6" s="32"/>
+      <c r="H6" s="33"/>
     </row>
     <row r="7" spans="2:8" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="19" t="s">
@@ -1554,7 +1554,7 @@
       </c>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B8" s="57" t="s">
+      <c r="B8" s="58" t="s">
         <v>0</v>
       </c>
       <c r="C8" s="3" t="s">
@@ -1577,12 +1577,12 @@
       </c>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B9" s="58"/>
+      <c r="B9" s="59"/>
       <c r="C9" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D9" s="45"/>
-      <c r="E9" s="46"/>
+      <c r="D9" s="46"/>
+      <c r="E9" s="47"/>
       <c r="F9" s="2" t="s">
         <v>74</v>
       </c>
@@ -1594,7 +1594,7 @@
       </c>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B10" s="34" t="s">
+      <c r="B10" s="35" t="s">
         <v>63</v>
       </c>
       <c r="C10" s="2" t="s">
@@ -1617,7 +1617,7 @@
       </c>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B11" s="34"/>
+      <c r="B11" s="35"/>
       <c r="C11" s="2" t="s">
         <v>50</v>
       </c>
@@ -1638,7 +1638,7 @@
       </c>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B12" s="34"/>
+      <c r="B12" s="35"/>
       <c r="C12" s="2" t="s">
         <v>5</v>
       </c>
@@ -1659,7 +1659,7 @@
       </c>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B13" s="34"/>
+      <c r="B13" s="35"/>
       <c r="C13" s="2" t="s">
         <v>2</v>
       </c>
@@ -1678,7 +1678,7 @@
       <c r="H13" s="8"/>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B14" s="34"/>
+      <c r="B14" s="35"/>
       <c r="C14" s="2" t="s">
         <v>3</v>
       </c>
@@ -1697,7 +1697,7 @@
       <c r="H14" s="8"/>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B15" s="34"/>
+      <c r="B15" s="35"/>
       <c r="C15" s="2" t="s">
         <v>4</v>
       </c>
@@ -1716,7 +1716,7 @@
       <c r="H15" s="8"/>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B16" s="34"/>
+      <c r="B16" s="35"/>
       <c r="C16" s="2" t="s">
         <v>11</v>
       </c>
@@ -1737,7 +1737,7 @@
       </c>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B17" s="34"/>
+      <c r="B17" s="35"/>
       <c r="C17" s="4" t="s">
         <v>20</v>
       </c>
@@ -1756,11 +1756,11 @@
       <c r="H17" s="8"/>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B18" s="34"/>
+      <c r="B18" s="35"/>
       <c r="C18" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D18" s="59">
+      <c r="D18" s="30">
         <v>0.03</v>
       </c>
       <c r="E18" s="5">
@@ -1777,7 +1777,7 @@
       </c>
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B19" s="35"/>
+      <c r="B19" s="36"/>
       <c r="C19" s="2" t="s">
         <v>18</v>
       </c>
@@ -1796,7 +1796,7 @@
       <c r="H19" s="8"/>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B20" s="33" t="s">
+      <c r="B20" s="34" t="s">
         <v>21</v>
       </c>
       <c r="C20" s="2" t="s">
@@ -1817,7 +1817,7 @@
       <c r="H20" s="8"/>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B21" s="34"/>
+      <c r="B21" s="35"/>
       <c r="C21" s="2" t="s">
         <v>25</v>
       </c>
@@ -1835,7 +1835,7 @@
       </c>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B22" s="34"/>
+      <c r="B22" s="35"/>
       <c r="C22" s="2" t="s">
         <v>58</v>
       </c>
@@ -1854,7 +1854,7 @@
       <c r="H22" s="8"/>
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B23" s="34"/>
+      <c r="B23" s="35"/>
       <c r="C23" s="2" t="s">
         <v>26</v>
       </c>
@@ -1875,7 +1875,7 @@
       </c>
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B24" s="34"/>
+      <c r="B24" s="35"/>
       <c r="C24" s="2" t="s">
         <v>29</v>
       </c>
@@ -1894,7 +1894,7 @@
       <c r="H24" s="8"/>
     </row>
     <row r="25" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B25" s="34"/>
+      <c r="B25" s="35"/>
       <c r="C25" s="2" t="s">
         <v>28</v>
       </c>
@@ -1913,7 +1913,7 @@
       <c r="H25" s="8"/>
     </row>
     <row r="26" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B26" s="34"/>
+      <c r="B26" s="35"/>
       <c r="C26" s="2" t="s">
         <v>27</v>
       </c>
@@ -1932,7 +1932,7 @@
       <c r="H26" s="8"/>
     </row>
     <row r="27" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B27" s="35"/>
+      <c r="B27" s="36"/>
       <c r="C27" s="2" t="s">
         <v>30</v>
       </c>
@@ -1951,7 +1951,7 @@
       <c r="H27" s="8"/>
     </row>
     <row r="28" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B28" s="33" t="s">
+      <c r="B28" s="34" t="s">
         <v>37</v>
       </c>
       <c r="C28" s="2" t="s">
@@ -1974,7 +1974,7 @@
       </c>
     </row>
     <row r="29" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B29" s="35"/>
+      <c r="B29" s="36"/>
       <c r="C29" s="2" t="s">
         <v>36</v>
       </c>
@@ -2014,13 +2014,13 @@
       <c r="H30" s="8"/>
     </row>
     <row r="31" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B31" s="33" t="s">
+      <c r="B31" s="34" t="s">
         <v>33</v>
       </c>
       <c r="C31" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="D31" s="59">
+      <c r="D31" s="30">
         <v>0.86</v>
       </c>
       <c r="E31" s="15">
@@ -2035,7 +2035,7 @@
       <c r="H31" s="8"/>
     </row>
     <row r="32" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B32" s="34"/>
+      <c r="B32" s="35"/>
       <c r="C32" s="2" t="s">
         <v>42</v>
       </c>
@@ -2054,7 +2054,7 @@
       <c r="H32" s="8"/>
     </row>
     <row r="33" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B33" s="35"/>
+      <c r="B33" s="36"/>
       <c r="C33" s="2" t="s">
         <v>55</v>
       </c>
@@ -2073,7 +2073,7 @@
       <c r="H33" s="8"/>
     </row>
     <row r="34" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B34" s="33" t="s">
+      <c r="B34" s="34" t="s">
         <v>61</v>
       </c>
       <c r="C34" s="2" t="s">
@@ -2082,123 +2082,123 @@
       <c r="D34" s="2">
         <v>8</v>
       </c>
-      <c r="E34" s="36"/>
-      <c r="F34" s="37"/>
-      <c r="G34" s="38"/>
+      <c r="E34" s="37"/>
+      <c r="F34" s="38"/>
+      <c r="G34" s="39"/>
       <c r="H34" s="8"/>
     </row>
     <row r="35" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B35" s="34"/>
+      <c r="B35" s="35"/>
       <c r="C35" s="2" t="s">
         <v>60</v>
       </c>
       <c r="D35" s="2">
         <v>6</v>
       </c>
-      <c r="E35" s="39"/>
-      <c r="F35" s="40"/>
-      <c r="G35" s="41"/>
+      <c r="E35" s="40"/>
+      <c r="F35" s="41"/>
+      <c r="G35" s="42"/>
       <c r="H35" s="8" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="36" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B36" s="35"/>
+      <c r="B36" s="36"/>
       <c r="C36" s="2" t="s">
         <v>59</v>
       </c>
       <c r="D36" s="2">
         <v>7</v>
       </c>
-      <c r="E36" s="42"/>
-      <c r="F36" s="43"/>
-      <c r="G36" s="44"/>
+      <c r="E36" s="43"/>
+      <c r="F36" s="44"/>
+      <c r="G36" s="45"/>
       <c r="H36" s="8"/>
     </row>
     <row r="37" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B37" s="33" t="s">
+      <c r="B37" s="34" t="s">
         <v>62</v>
       </c>
-      <c r="C37" s="48" t="s">
+      <c r="C37" s="49" t="s">
         <v>89</v>
       </c>
-      <c r="D37" s="49"/>
-      <c r="E37" s="49"/>
-      <c r="F37" s="49"/>
-      <c r="G37" s="49"/>
-      <c r="H37" s="50"/>
+      <c r="D37" s="50"/>
+      <c r="E37" s="50"/>
+      <c r="F37" s="50"/>
+      <c r="G37" s="50"/>
+      <c r="H37" s="51"/>
     </row>
     <row r="38" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B38" s="34"/>
-      <c r="C38" s="51"/>
-      <c r="D38" s="52"/>
-      <c r="E38" s="52"/>
-      <c r="F38" s="52"/>
-      <c r="G38" s="52"/>
-      <c r="H38" s="53"/>
+      <c r="B38" s="35"/>
+      <c r="C38" s="52"/>
+      <c r="D38" s="53"/>
+      <c r="E38" s="53"/>
+      <c r="F38" s="53"/>
+      <c r="G38" s="53"/>
+      <c r="H38" s="54"/>
     </row>
     <row r="39" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B39" s="34"/>
-      <c r="C39" s="51"/>
-      <c r="D39" s="52"/>
-      <c r="E39" s="52"/>
-      <c r="F39" s="52"/>
-      <c r="G39" s="52"/>
-      <c r="H39" s="53"/>
+      <c r="B39" s="35"/>
+      <c r="C39" s="52"/>
+      <c r="D39" s="53"/>
+      <c r="E39" s="53"/>
+      <c r="F39" s="53"/>
+      <c r="G39" s="53"/>
+      <c r="H39" s="54"/>
     </row>
     <row r="40" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B40" s="34"/>
-      <c r="C40" s="51"/>
-      <c r="D40" s="52"/>
-      <c r="E40" s="52"/>
-      <c r="F40" s="52"/>
-      <c r="G40" s="52"/>
-      <c r="H40" s="53"/>
+      <c r="B40" s="35"/>
+      <c r="C40" s="52"/>
+      <c r="D40" s="53"/>
+      <c r="E40" s="53"/>
+      <c r="F40" s="53"/>
+      <c r="G40" s="53"/>
+      <c r="H40" s="54"/>
     </row>
     <row r="41" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B41" s="34"/>
-      <c r="C41" s="51"/>
-      <c r="D41" s="52"/>
-      <c r="E41" s="52"/>
-      <c r="F41" s="52"/>
-      <c r="G41" s="52"/>
-      <c r="H41" s="53"/>
+      <c r="B41" s="35"/>
+      <c r="C41" s="52"/>
+      <c r="D41" s="53"/>
+      <c r="E41" s="53"/>
+      <c r="F41" s="53"/>
+      <c r="G41" s="53"/>
+      <c r="H41" s="54"/>
     </row>
     <row r="42" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B42" s="34"/>
-      <c r="C42" s="51"/>
-      <c r="D42" s="52"/>
-      <c r="E42" s="52"/>
-      <c r="F42" s="52"/>
-      <c r="G42" s="52"/>
-      <c r="H42" s="53"/>
+      <c r="B42" s="35"/>
+      <c r="C42" s="52"/>
+      <c r="D42" s="53"/>
+      <c r="E42" s="53"/>
+      <c r="F42" s="53"/>
+      <c r="G42" s="53"/>
+      <c r="H42" s="54"/>
     </row>
     <row r="43" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B43" s="34"/>
-      <c r="C43" s="51"/>
-      <c r="D43" s="52"/>
-      <c r="E43" s="52"/>
-      <c r="F43" s="52"/>
-      <c r="G43" s="52"/>
-      <c r="H43" s="53"/>
+      <c r="B43" s="35"/>
+      <c r="C43" s="52"/>
+      <c r="D43" s="53"/>
+      <c r="E43" s="53"/>
+      <c r="F43" s="53"/>
+      <c r="G43" s="53"/>
+      <c r="H43" s="54"/>
     </row>
     <row r="44" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B44" s="34"/>
-      <c r="C44" s="51"/>
-      <c r="D44" s="52"/>
-      <c r="E44" s="52"/>
-      <c r="F44" s="52"/>
-      <c r="G44" s="52"/>
-      <c r="H44" s="53"/>
+      <c r="B44" s="35"/>
+      <c r="C44" s="52"/>
+      <c r="D44" s="53"/>
+      <c r="E44" s="53"/>
+      <c r="F44" s="53"/>
+      <c r="G44" s="53"/>
+      <c r="H44" s="54"/>
     </row>
     <row r="45" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B45" s="47"/>
-      <c r="C45" s="54"/>
-      <c r="D45" s="55"/>
-      <c r="E45" s="55"/>
-      <c r="F45" s="55"/>
-      <c r="G45" s="55"/>
-      <c r="H45" s="56"/>
+      <c r="B45" s="48"/>
+      <c r="C45" s="55"/>
+      <c r="D45" s="56"/>
+      <c r="E45" s="56"/>
+      <c r="F45" s="56"/>
+      <c r="G45" s="56"/>
+      <c r="H45" s="57"/>
     </row>
   </sheetData>
   <mergeCells count="11">

</xml_diff>